<commit_message>
excel built-in number format 설정
</commit_message>
<xml_diff>
--- a/Common/utils/codegen/test/xlsx_numformat/input.xlsx
+++ b/Common/utils/codegen/test/xlsx_numformat/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\utils\codegen\test\xlsx_numformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C83D95D-1B73-4D70-A054-E0E2FDCF26D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F663246-A957-4BB6-B46A-BCFFD96D5A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5190" yWindow="1245" windowWidth="20310" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,89 +33,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>NUMFORMAT_NUMBER_D2</t>
   </si>
   <si>
+    <t>NUMFORMAT_CURRENCY_NEGBRA</t>
+  </si>
+  <si>
+    <t>NUMFORMAT_PERCENT</t>
+  </si>
+  <si>
+    <t>NUMFORMAT_SCIENTIFIC_D2</t>
+  </si>
+  <si>
+    <t>NUMFORMAT_FRACTION_ONEDIG</t>
+  </si>
+  <si>
+    <t>NUMFORMAT_DATE</t>
+  </si>
+  <si>
+    <t>NUMFORMAT_CUSTOM_MON_YY</t>
+  </si>
+  <si>
+    <t>#.###</t>
+  </si>
+  <si>
+    <t>#.00</t>
+  </si>
+  <si>
+    <t>0.00 "dollars"</t>
+  </si>
+  <si>
+    <t>[Red][&lt;=100];[Green][&gt;100]</t>
+  </si>
+  <si>
+    <t>= 2.57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= -25%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 8.90E+02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 3/4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 2020-05-16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= May-20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 20.563</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 4.80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 1.23 dollars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 60 (red)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= -₩500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMFORMAT_NUMBER_SEP_D2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>NUMFORMAT_NUMBER_SEP</t>
-  </si>
-  <si>
-    <t>NUMFORMAT_CURRENCY_NEGBRA</t>
-  </si>
-  <si>
-    <t>NUMFORMAT_PERCENT</t>
-  </si>
-  <si>
-    <t>NUMFORMAT_SCIENTIFIC_D2</t>
-  </si>
-  <si>
-    <t>NUMFORMAT_FRACTION_ONEDIG</t>
-  </si>
-  <si>
-    <t>NUMFORMAT_DATE</t>
-  </si>
-  <si>
-    <t>NUMFORMAT_CUSTOM_MON_YY</t>
-  </si>
-  <si>
-    <t>#.###</t>
-  </si>
-  <si>
-    <t>#.00</t>
-  </si>
-  <si>
-    <t>0.00 "dollars"</t>
-  </si>
-  <si>
-    <t>[Red][&lt;=100];[Green][&gt;100]</t>
-  </si>
-  <si>
-    <t>= 2.57</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= 2,500,000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= -25%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= 8.90E+02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= 3/4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= 2020-05-16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= May-20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= 20.563</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= 4.80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= 1.23 dollars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= 60 (red)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>= -₩500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 2,500,001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 123,000.65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMFORMAT_FRACTION_TWODIG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 3  7/40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 1/8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMFORMAT_FRACTION_8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -123,12 +148,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="5" formatCode="&quot;₩&quot;#,##0;\-&quot;₩&quot;#,##0"/>
     <numFmt numFmtId="176" formatCode="#.###"/>
     <numFmt numFmtId="177" formatCode="#.00"/>
     <numFmt numFmtId="178" formatCode="0.00\ &quot;dollars&quot;"/>
     <numFmt numFmtId="179" formatCode="[Red][&lt;=100]General;[Green][&gt;100]General"/>
+    <numFmt numFmtId="180" formatCode="#\ ?/8"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -251,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -266,6 +292,10 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="13" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -600,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,132 +651,166 @@
         <v>2.5680999999999998</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="B2" s="2">
-        <v>2500000</v>
+        <v>2500000.5</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>-500</v>
+      <c r="A3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="15">
+        <v>123000.6452</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4">
-        <v>-0.25</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-500</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>890</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>-0.25</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0.75</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>890</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7">
-        <v>43967</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.75</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8">
-        <v>43967</v>
+      <c r="A8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="16">
+        <v>3.1749999999999998</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9">
-        <v>20.5627</v>
+      <c r="A9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="17">
+        <v>0.17499999999999999</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10">
-        <v>4.8</v>
+        <v>5</v>
+      </c>
+      <c r="B10" s="7">
+        <v>43967</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11">
-        <v>1.23</v>
+        <v>6</v>
+      </c>
+      <c r="B11" s="8">
+        <v>43967</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="12">
+        <v>7</v>
+      </c>
+      <c r="B12" s="9">
+        <v>20.5627</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="10">
+        <v>4.8</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1.23</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="12">
         <v>60</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>22</v>
+      <c r="C15" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docgen excel 에 number format 추가
</commit_message>
<xml_diff>
--- a/Common/utils/codegen/test/xlsx_numformat/input.xlsx
+++ b/Common/utils/codegen/test/xlsx_numformat/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\utils\codegen\test\xlsx_numformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F663246-A957-4BB6-B46A-BCFFD96D5A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E926D1-3F5B-4E25-A425-B1163EE500D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="1245" windowWidth="20310" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,10 +104,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>= 60 (red)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>= -₩500</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -141,6 +137,10 @@
   </si>
   <si>
     <t>NUMFORMAT_FRACTION_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>= 160 (green)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -633,7 +633,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,24 +656,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2">
         <v>2500000.5</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="15">
         <v>123000.6452</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>-500</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -722,24 +722,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="16">
         <v>3.1749999999999998</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="17">
         <v>0.17499999999999999</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -802,10 +802,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="12">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>